<commit_message>
10001 - 10004 加入特效
</commit_message>
<xml_diff>
--- a/Config/Datas/EffectData.xlsx
+++ b/Config/Datas/EffectData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goho/Documents/GitHub/goblin/Config/Datas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EEDDED-1974-B644-BAFB-7EE167AF6B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3A5AD4-FD37-CC4E-96E2-D7B3E2B2D8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>##var</t>
   </si>
@@ -65,6 +65,22 @@
   </si>
   <si>
     <t>Effect_Sword_Slash_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>刀光-蓝色-旋转</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect_Sword_Slash_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>刀光-浅蓝色-力量竖劈</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect_Sword_Slash_3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -479,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -545,6 +561,28 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="2">
+        <v>1000002</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="2">
+        <v>1000003</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>